<commit_message>
Fixed formatting in spreadsheet
</commit_message>
<xml_diff>
--- a/DEPNotify User Input Registration Preference Keys.xlsx
+++ b/DEPNotify User Input Registration Preference Keys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11202"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fdeis/Documents/AgileMobility360/Infrastructure/Xcode Projects/DEPNotify/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyle/GitHub/DEPNotify-App/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{B9AB3197-9409-E747-8E21-35AC699F8A15}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{19EDAC77-133D-B146-83C4-F4C1D3FFA5D7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="460" windowWidth="28020" windowHeight="17380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -18,6 +18,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <customWorkbookViews>
+    <customWorkbookView name="Kyle Bareis - Personal View" guid="{44080EC3-1562-1A4B-B8E3-C7D88D63F19E}" mergeInterval="0" personalView="1" maximized="1" yWindow="23" windowWidth="1920" windowHeight="984" activeSheetId="2"/>
     <customWorkbookView name="Federico Deis - Personal View" guid="{9FC80166-3721-9A4D-A675-78A688924A11}" mergeInterval="0" personalView="1" xWindow="28" yWindow="23" windowWidth="1401" windowHeight="869" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
@@ -697,7 +698,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -706,7 +707,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -726,6 +726,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -744,7 +748,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{53912F80-C8BD-774C-A118-C54A08DB7462}" diskRevisions="1" revisionId="257" version="8">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{AE6E0D60-3335-1D4C-8CE7-E09E2B1D01EA}" diskRevisions="1" revisionId="257" version="9">
   <header guid="{DEA7F92A-108D-094D-97A2-1B0ED6494E8D}" dateTime="2018-11-27T15:57:34" maxSheetId="3" userName="Federico Deis" r:id="rId5" minRId="195" maxRId="197">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -764,6 +768,12 @@
     </sheetIdMap>
   </header>
   <header guid="{53912F80-C8BD-774C-A118-C54A08DB7462}" dateTime="2018-12-12T20:00:43" maxSheetId="3" userName="Federico Deis" r:id="rId8" minRId="248" maxRId="257">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{AE6E0D60-3335-1D4C-8CE7-E09E2B1D01EA}" dateTime="2019-01-08T09:41:31" maxSheetId="3" userName="Kyle Bareis" r:id="rId9">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -985,6 +995,26 @@
       </is>
     </nc>
   </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="2" sqref="B36" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <sz val="11"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="2" sqref="A3:F41" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <sz val="11"/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcv guid="{44080EC3-1562-1A4B-B8E3-C7D88D63F19E}" action="add"/>
 </revisions>
 </file>
 
@@ -2326,6 +2356,11 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{44080EC3-1562-1A4B-B8E3-C7D88D63F19E}" state="hidden" topLeftCell="A12">
+      <selection activeCell="B25" sqref="B25"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+    </customSheetView>
     <customSheetView guid="{9FC80166-3721-9A4D-A675-78A688924A11}" state="hidden" topLeftCell="A12">
       <selection activeCell="B25" sqref="B25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2341,8 +2376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E3AB8B7-C63D-3E45-856D-77E679403626}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2360,53 +2395,53 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:6" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="12"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="13" t="s">
         <v>139</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:6" s="9" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -2448,15 +2483,15 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:6" s="9" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
@@ -2648,7 +2683,7 @@
       <c r="C18" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>174</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -2668,7 +2703,7 @@
       <c r="C19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>175</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -2794,7 +2829,7 @@
       <c r="E25" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="6" t="s">
         <v>157</v>
       </c>
     </row>
@@ -2814,7 +2849,7 @@
       <c r="E26" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="6" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3002,7 +3037,7 @@
       <c r="A36" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="5" t="s">
         <v>187</v>
       </c>
       <c r="C36" s="5" t="s">
@@ -3014,90 +3049,98 @@
       <c r="E36" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="5" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="9" t="s">
+    <row r="37" spans="1:6" s="9" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
     </row>
     <row r="38" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="1" t="s">
+      <c r="A38" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="C38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="5" t="s">
         <v>68</v>
       </c>
+      <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" s="1" t="s">
+      <c r="A39" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="C39" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="5" t="s">
         <v>69</v>
       </c>
+      <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" s="1" t="s">
+      <c r="A40" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="1" t="s">
+      <c r="C40" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="1" t="s">
+      <c r="A41" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="5" t="s">
         <v>52</v>
       </c>
+      <c r="F41" s="5"/>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{44080EC3-1562-1A4B-B8E3-C7D88D63F19E}" topLeftCell="A20">
+      <selection activeCell="D28" sqref="D28"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{9FC80166-3721-9A4D-A675-78A688924A11}" topLeftCell="A2">
       <selection activeCell="D17" sqref="D17"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>